<commit_message>
update xlsx file and adding instructions
</commit_message>
<xml_diff>
--- a/8. Final Project/Risk Fracture Calculation.xlsx
+++ b/8. Final Project/Risk Fracture Calculation.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="15">
   <si>
     <t>TOTAL</t>
   </si>
@@ -56,6 +56,13 @@
   </si>
   <si>
     <t>Patient ID_4532</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* The first row of the table ("Days after the first X-ray") shows the days that have passed since each of the radiographs were taken until the day the probability study was carried out. In the Patient ID_4532 the probability study starts 14 days after the 24 months X-Ray was taken. In addition, the last column shows the total days passed from the first radiography.
+* In the next row, the number of days value is divided by the total of days, obtaining the weights assigned to the days passed. In this case, the total weights are also obtained adding all the values of the second row.
+* In the third row, the same idea is followed than in the second row because the result value that is needed must be between 0-1.                                          * EMD row is the EMD values obtained from the programming code with the radiographs.
+* In the next row, the sum of the EMD is divided between each EMD value, obtaining the weight of the Earth mover´s distance.                       * The probability is calculated multiplying the row "Ponderation of days" by "EMD weight". 
+* Finally, the probability of hip fracture is obtained as an artithmetic mean of these probabilities, and multiplied by 100 to express it as a percentage.                                                                                              </t>
   </si>
 </sst>
 </file>
@@ -67,7 +74,7 @@
     <numFmt numFmtId="165" formatCode="#,##0.00000000"/>
     <numFmt numFmtId="166" formatCode="#,##0.0000000000000000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -89,6 +96,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="5">
@@ -117,7 +130,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -253,6 +266,86 @@
       </right>
       <top/>
       <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -262,7 +355,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -318,6 +411,33 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -621,11 +741,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:G22"/>
+  <dimension ref="B1:M22"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -633,7 +751,8 @@
     <col min="3" max="7" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B2" s="4" t="s">
         <v>13</v>
       </c>
@@ -652,8 +771,15 @@
       <c r="G2" s="5" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I2" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="J2" s="23"/>
+      <c r="K2" s="23"/>
+      <c r="L2" s="23"/>
+      <c r="M2" s="24"/>
+    </row>
+    <row r="3" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B3" s="17" t="s">
         <v>11</v>
       </c>
@@ -673,8 +799,13 @@
         <f>SUM(D3:F3)</f>
         <v>599</v>
       </c>
-    </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I3" s="25"/>
+      <c r="J3" s="26"/>
+      <c r="K3" s="26"/>
+      <c r="L3" s="26"/>
+      <c r="M3" s="27"/>
+    </row>
+    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B4" s="18" t="s">
         <v>2</v>
       </c>
@@ -697,8 +828,13 @@
         <f>SUM(D4:F4)</f>
         <v>47.325709621535182</v>
       </c>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I4" s="25"/>
+      <c r="J4" s="26"/>
+      <c r="K4" s="26"/>
+      <c r="L4" s="26"/>
+      <c r="M4" s="27"/>
+    </row>
+    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B5" s="18" t="s">
         <v>12</v>
       </c>
@@ -718,16 +854,26 @@
         <v>0.90406915454353776</v>
       </c>
       <c r="G5" s="11"/>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I5" s="25"/>
+      <c r="J5" s="26"/>
+      <c r="K5" s="26"/>
+      <c r="L5" s="26"/>
+      <c r="M5" s="27"/>
+    </row>
+    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B6" s="18"/>
       <c r="C6" s="10"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="11"/>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I6" s="25"/>
+      <c r="J6" s="26"/>
+      <c r="K6" s="26"/>
+      <c r="L6" s="26"/>
+      <c r="M6" s="27"/>
+    </row>
+    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B7" s="19" t="s">
         <v>1</v>
       </c>
@@ -747,8 +893,13 @@
         <f>SUM(D7:F7)</f>
         <v>256.75307488314434</v>
       </c>
-    </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I7" s="25"/>
+      <c r="J7" s="26"/>
+      <c r="K7" s="26"/>
+      <c r="L7" s="26"/>
+      <c r="M7" s="27"/>
+    </row>
+    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B8" s="18" t="s">
         <v>8</v>
       </c>
@@ -768,16 +919,26 @@
         <v>0.43518067448351427</v>
       </c>
       <c r="G8" s="11"/>
-    </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I8" s="25"/>
+      <c r="J8" s="26"/>
+      <c r="K8" s="26"/>
+      <c r="L8" s="26"/>
+      <c r="M8" s="27"/>
+    </row>
+    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B9" s="18"/>
       <c r="C9" s="12"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
       <c r="G9" s="11"/>
-    </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I9" s="25"/>
+      <c r="J9" s="26"/>
+      <c r="K9" s="26"/>
+      <c r="L9" s="26"/>
+      <c r="M9" s="27"/>
+    </row>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B10" s="20" t="s">
         <v>9</v>
       </c>
@@ -795,8 +956,13 @@
         <v>0.39343342445399726</v>
       </c>
       <c r="G10" s="16"/>
-    </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I10" s="25"/>
+      <c r="J10" s="26"/>
+      <c r="K10" s="26"/>
+      <c r="L10" s="26"/>
+      <c r="M10" s="27"/>
+    </row>
+    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B11" s="4" t="s">
         <v>10</v>
       </c>
@@ -808,8 +974,20 @@
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
-    </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I11" s="25"/>
+      <c r="J11" s="26"/>
+      <c r="K11" s="26"/>
+      <c r="L11" s="26"/>
+      <c r="M11" s="27"/>
+    </row>
+    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="I12" s="25"/>
+      <c r="J12" s="26"/>
+      <c r="K12" s="26"/>
+      <c r="L12" s="26"/>
+      <c r="M12" s="27"/>
+    </row>
+    <row r="13" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B13" s="4" t="s">
         <v>13</v>
       </c>
@@ -828,8 +1006,13 @@
       <c r="G13" s="5" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I13" s="25"/>
+      <c r="J13" s="26"/>
+      <c r="K13" s="26"/>
+      <c r="L13" s="26"/>
+      <c r="M13" s="27"/>
+    </row>
+    <row r="14" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B14" s="17" t="s">
         <v>11</v>
       </c>
@@ -849,8 +1032,13 @@
         <f>SUM(C14:F14)</f>
         <v>1169</v>
       </c>
-    </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I14" s="25"/>
+      <c r="J14" s="26"/>
+      <c r="K14" s="26"/>
+      <c r="L14" s="26"/>
+      <c r="M14" s="27"/>
+    </row>
+    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B15" s="18" t="s">
         <v>2</v>
       </c>
@@ -874,8 +1062,13 @@
         <f>SUM(C15:F15)</f>
         <v>38.869880254910264</v>
       </c>
-    </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I15" s="25"/>
+      <c r="J15" s="26"/>
+      <c r="K15" s="26"/>
+      <c r="L15" s="26"/>
+      <c r="M15" s="27"/>
+    </row>
+    <row r="16" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B16" s="18" t="s">
         <v>12</v>
       </c>
@@ -896,16 +1089,26 @@
         <v>0.85613275779448639</v>
       </c>
       <c r="G16" s="11"/>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I16" s="25"/>
+      <c r="J16" s="26"/>
+      <c r="K16" s="26"/>
+      <c r="L16" s="26"/>
+      <c r="M16" s="27"/>
+    </row>
+    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B17" s="18"/>
       <c r="C17" s="10"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="G17" s="11"/>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I17" s="25"/>
+      <c r="J17" s="26"/>
+      <c r="K17" s="26"/>
+      <c r="L17" s="26"/>
+      <c r="M17" s="27"/>
+    </row>
+    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B18" s="19" t="s">
         <v>1</v>
       </c>
@@ -925,8 +1128,13 @@
         <f>SUM(C18:F18)</f>
         <v>165.21418275882178</v>
       </c>
-    </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I18" s="25"/>
+      <c r="J18" s="26"/>
+      <c r="K18" s="26"/>
+      <c r="L18" s="26"/>
+      <c r="M18" s="27"/>
+    </row>
+    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B19" s="18" t="s">
         <v>8</v>
       </c>
@@ -947,16 +1155,26 @@
         <v>0.32798056770170375</v>
       </c>
       <c r="G19" s="11"/>
-    </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I19" s="25"/>
+      <c r="J19" s="26"/>
+      <c r="K19" s="26"/>
+      <c r="L19" s="26"/>
+      <c r="M19" s="27"/>
+    </row>
+    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B20" s="18"/>
       <c r="C20" s="12"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="G20" s="11"/>
-    </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I20" s="25"/>
+      <c r="J20" s="26"/>
+      <c r="K20" s="26"/>
+      <c r="L20" s="26"/>
+      <c r="M20" s="27"/>
+    </row>
+    <row r="21" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" s="20" t="s">
         <v>9</v>
       </c>
@@ -977,8 +1195,13 @@
         <v>0.28079490792946088</v>
       </c>
       <c r="G21" s="16"/>
-    </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I21" s="28"/>
+      <c r="J21" s="29"/>
+      <c r="K21" s="29"/>
+      <c r="L21" s="29"/>
+      <c r="M21" s="30"/>
+    </row>
+    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B22" s="4" t="s">
         <v>10</v>
       </c>
@@ -992,6 +1215,10 @@
       <c r="G22" s="1"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="I2:M21"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
last revisions of the final project
</commit_message>
<xml_diff>
--- a/8. Final Project/Risk Fracture Calculation.xlsx
+++ b/8. Final Project/Risk Fracture Calculation.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="16">
   <si>
     <t>TOTAL</t>
   </si>
@@ -63,6 +63,9 @@
 * In the third row, the same idea is followed than in the second row because the result value that is needed must be between 0-1.                                          * EMD row is the EMD values obtained from the programming code with the radiographs.
 * In the next row, the sum of the EMD is divided between each EMD value, obtaining the weight of the Earth mover´s distance.                       * The probability is calculated multiplying the row "Ponderation of days" by "EMD weight". 
 * Finally, the probability of hip fracture is obtained as an artithmetic mean of these probabilities, and multiplied by 100 to express it as a percentage.                                                                                              </t>
+  </si>
+  <si>
+    <t>Function weight days [0-1]</t>
   </si>
 </sst>
 </file>
@@ -743,11 +746,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:M22"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="7" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -836,7 +841,7 @@
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B5" s="18" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C5" s="10" t="s">
         <v>7</v>
@@ -881,17 +886,17 @@
         <v>7</v>
       </c>
       <c r="D7" s="3">
-        <v>66.784329618523699</v>
+        <v>439.39234016021902</v>
       </c>
       <c r="E7" s="3">
-        <v>78.2347689612576</v>
+        <v>654.28872805784101</v>
       </c>
       <c r="F7" s="3">
-        <v>111.73397630336299</v>
+        <v>702.68683785809503</v>
       </c>
       <c r="G7" s="13">
         <f>SUM(D7:F7)</f>
-        <v>256.75307488314434</v>
+        <v>1796.3679060761551</v>
       </c>
       <c r="I7" s="25"/>
       <c r="J7" s="26"/>
@@ -908,15 +913,15 @@
       </c>
       <c r="D8" s="2">
         <f>D7/$G7</f>
-        <v>0.26011111901549439</v>
+        <v>0.24460041769505508</v>
       </c>
       <c r="E8" s="2">
         <f>E7/$G7</f>
-        <v>0.30470820650099117</v>
+        <v>0.36422868937077479</v>
       </c>
       <c r="F8" s="2">
         <f>F7/$G7</f>
-        <v>0.43518067448351427</v>
+        <v>0.39117089293417012</v>
       </c>
       <c r="G8" s="11"/>
       <c r="I8" s="25"/>
@@ -945,15 +950,15 @@
       <c r="C10" s="14"/>
       <c r="D10" s="15">
         <f>D5*D8</f>
-        <v>8.573484771822815E-3</v>
+        <v>8.0622388009685027E-3</v>
       </c>
       <c r="E10" s="15">
         <f>E5*E8</f>
-        <v>1.9187472979470665E-2</v>
+        <v>2.2935477241985681E-2</v>
       </c>
       <c r="F10" s="15">
         <f>F5*F8</f>
-        <v>0.39343342445399726</v>
+        <v>0.35364553845703589</v>
       </c>
       <c r="G10" s="16"/>
       <c r="I10" s="25"/>
@@ -968,7 +973,7 @@
       </c>
       <c r="C11" s="6">
         <f>AVERAGE(D10:F10)</f>
-        <v>0.14039812740176358</v>
+        <v>0.12821441816666337</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
@@ -1113,20 +1118,20 @@
         <v>1</v>
       </c>
       <c r="C18" s="21">
-        <v>28.4158694851794</v>
+        <v>70.436045094786607</v>
       </c>
       <c r="D18" s="3">
-        <v>35.008388166839701</v>
+        <v>74.826132426441106</v>
       </c>
       <c r="E18" s="3">
-        <v>47.602883653191299</v>
+        <v>114.872977309681</v>
       </c>
       <c r="F18" s="3">
-        <v>54.1870414536114</v>
+        <v>150.17002954437899</v>
       </c>
       <c r="G18" s="13">
         <f>SUM(C18:F18)</f>
-        <v>165.21418275882178</v>
+        <v>410.30518437528769</v>
       </c>
       <c r="I18" s="25"/>
       <c r="J18" s="26"/>
@@ -1140,19 +1145,19 @@
       </c>
       <c r="C19" s="21">
         <f>C18/$G18</f>
-        <v>0.17199412913999423</v>
+        <v>0.1716674509049389</v>
       </c>
       <c r="D19" s="2">
         <f>D18/$G18</f>
-        <v>0.21189699081673055</v>
+        <v>0.1823670167374756</v>
       </c>
       <c r="E19" s="2">
         <f>E18/$G18</f>
-        <v>0.2881283123415716</v>
+        <v>0.27996959747067651</v>
       </c>
       <c r="F19" s="2">
         <f>F18/$G18</f>
-        <v>0.32798056770170375</v>
+        <v>0.36599593488690901</v>
       </c>
       <c r="G19" s="11"/>
       <c r="I19" s="25"/>
@@ -1180,19 +1185,19 @@
       </c>
       <c r="C21" s="14">
         <f>C16*C19</f>
-        <v>4.6663671582597138E-3</v>
+        <v>4.657504061623784E-3</v>
       </c>
       <c r="D21" s="15">
         <f t="shared" ref="D21:F21" si="0">D16*D19</f>
-        <v>8.5706435488006535E-3</v>
+        <v>7.3762382820570828E-3</v>
       </c>
       <c r="E21" s="15">
         <f t="shared" si="0"/>
-        <v>2.1981037423692552E-2</v>
+        <v>2.1358616754758839E-2</v>
       </c>
       <c r="F21" s="15">
         <f t="shared" si="0"/>
-        <v>0.28079490792946088</v>
+        <v>0.31334110907630069</v>
       </c>
       <c r="G21" s="16"/>
       <c r="I21" s="28"/>
@@ -1207,7 +1212,7 @@
       </c>
       <c r="C22" s="6">
         <f>AVERAGE(C21:F21)</f>
-        <v>7.9003239015053447E-2</v>
+        <v>8.6683367043685094E-2</v>
       </c>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>

</xml_diff>